<commit_message>
add all formats files (yml, json, csv, md)
</commit_message>
<xml_diff>
--- a/converted-data/excel/listovki_page_03.xlsx
+++ b/converted-data/excel/listovki_page_03.xlsx
@@ -493,14 +493,14 @@
         <is>
           <t>✅ Звичайно! Першокласний європейський крейдований папір від 115 до 350г/м².
 💰 А5: 100 шт — від 280 грн ⚡ 1-2 дні, 💰 1000 шт збірним тиражем — 800 грн за ⚡ тиждень.
-Чи маєте готовий для друку макет?</t>
+❓ Чи маєте готовий для друку макет?</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
           <t>✅ Конечно! Первоклассная мелованная бумага от 115 до 350г/м².
 💰 А5: 100 шт — от 280 грн ⚡ 1-2 дня, 💰 1000 шт — от 850 грн. сборным тиражем за ⚡ неделю.
-Есть ли у вас макет, готовый к печати?</t>
+❓ Есть ли у вас макет, готовый к печати?</t>
         </is>
       </c>
       <c r="G2" t="n">

</xml_diff>